<commit_message>
50 data in spreadsheet and fixed some of the links.
</commit_message>
<xml_diff>
--- a/documents/IBM Reputation Economy - Datasheet - Clean - Revised.xlsx
+++ b/documents/IBM Reputation Economy - Datasheet - Clean - Revised.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IBM\Reputation Economy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IBM\Reputation-Economics-IBM-Intern-Project\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FF4754-EB42-4E10-953B-37177B1D5EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC0A089-2553-423B-88A6-8BB22C0FD644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5D8DA2A2-8BCE-49BD-9EEC-518A7BC766DC}"/>
   </bookViews>
@@ -1966,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C38B6D-0208-400D-B0AE-C75ADA3342BE}">
   <dimension ref="B2:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>